<commit_message>
Calificaciones a 25 de mayo de 2020.
</commit_message>
<xml_diff>
--- a/notasED/CalificacionesCod25demayo.xlsx
+++ b/notasED/CalificacionesCod25demayo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Konrad Lorenz\Asignaturas\2020-I\Estructuras de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE94BEB8-8387-4E7F-82BD-C7F8118E7935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{600D7AEF-C0CE-45E9-9020-30A572871F03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calificaciones Grupo 1" sheetId="1" r:id="rId1"/>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3385,7 +3385,9 @@
       <c r="V24" s="10">
         <v>5</v>
       </c>
-      <c r="W24" s="10"/>
+      <c r="W24" s="10">
+        <v>7</v>
+      </c>
       <c r="X24" s="10">
         <v>8</v>
       </c>
@@ -3397,7 +3399,7 @@
       </c>
       <c r="AA24" s="10">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="AB24" s="10">
         <f t="shared" si="1"/>
@@ -3405,7 +3407,7 @@
       </c>
       <c r="AC24" s="10">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AD24" s="15">
         <v>5</v>
@@ -3422,7 +3424,7 @@
       </c>
       <c r="AH24" s="18">
         <f t="shared" si="4"/>
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AI24" s="18">
         <f t="shared" si="5"/>
@@ -3430,7 +3432,7 @@
       </c>
       <c r="AJ24" s="19">
         <f t="shared" si="6"/>
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="AK24" s="19">
         <v>40</v>
@@ -3674,8 +3676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E37ED78-914C-4768-B352-F7C1A3B9BD7F}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>